<commit_message>
adding 2022 data and metadata
Added processed data for 2 of 3 markers from 2022 Eastern Shore Islands samples
#ESI
</commit_message>
<xml_diff>
--- a/data/2023Perley/2023_Perley_AlleDNA_Samples.xlsx
+++ b/data/2023Perley/2023_Perley_AlleDNA_Samples.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27630"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27720"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://086gc.sharepoint.com/sites/ABL-APC0259St.AnnsandESIMetabarcoding/Shared Documents/APC0259 St. Anns and ESI Metabarcoding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="360" documentId="13_ncr:1_{6E9B1B49-41D7-4A94-BB92-BABE92EEFB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA7DEF09-5949-453A-B88F-B4F7ED5A3687}"/>
+  <xr:revisionPtr revIDLastSave="390" documentId="13_ncr:1_{6E9B1B49-41D7-4A94-BB92-BABE92EEFB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CEF31C3-2392-44A1-9787-574FD31CA43D}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="25635" windowHeight="14445" xr2:uid="{1A36D6D2-5D1A-45A9-81DA-D9374A4D0A88}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="25635" windowHeight="14445" firstSheet="3" activeTab="3" xr2:uid="{1A36D6D2-5D1A-45A9-81DA-D9374A4D0A88}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4400" uniqueCount="517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4405" uniqueCount="517">
   <si>
     <t>station</t>
   </si>
@@ -1813,7 +1813,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -2162,11 +2162,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2291,6 +2326,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2300,14 +2337,24 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2635,7 +2682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCEF5612-4730-4E31-84E1-3CCD713AC1DF}">
   <dimension ref="A1:U208"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H182" sqref="H182"/>
     </sheetView>
@@ -10103,7 +10150,7 @@
       <c r="G134" t="s">
         <v>324</v>
       </c>
-      <c r="H134" s="125">
+      <c r="H134" s="31">
         <v>413425</v>
       </c>
       <c r="I134" t="s">
@@ -10263,7 +10310,7 @@
       <c r="G137" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="H137" s="126">
+      <c r="H137" s="39">
         <v>413428</v>
       </c>
       <c r="I137" s="10" t="s">
@@ -10429,7 +10476,7 @@
       <c r="G140" t="s">
         <v>334</v>
       </c>
-      <c r="H140" s="125">
+      <c r="H140" s="31">
         <v>413431</v>
       </c>
       <c r="I140" t="s">
@@ -10645,7 +10692,7 @@
       <c r="G144" t="s">
         <v>348</v>
       </c>
-      <c r="H144" s="125">
+      <c r="H144" s="31">
         <v>413435</v>
       </c>
       <c r="I144" t="s">
@@ -11722,7 +11769,7 @@
       <c r="G163" t="s">
         <v>395</v>
       </c>
-      <c r="H163" s="125">
+      <c r="H163" s="31">
         <v>413454</v>
       </c>
       <c r="I163" t="s">
@@ -12112,7 +12159,7 @@
       <c r="G170" t="s">
         <v>104</v>
       </c>
-      <c r="H170" s="125">
+      <c r="H170" s="31">
         <v>413461</v>
       </c>
       <c r="I170" t="s">
@@ -12788,7 +12835,7 @@
       <c r="G182" t="s">
         <v>440</v>
       </c>
-      <c r="H182" s="125">
+      <c r="H182" s="31">
         <v>413473</v>
       </c>
       <c r="I182" t="s">
@@ -18108,8 +18155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F7599B-F915-4321-A886-3CB05A310A40}">
   <dimension ref="A1:Y121"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="O80" sqref="O80:O81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18176,15 +18223,15 @@
       </c>
       <c r="Q1" s="31"/>
       <c r="R1" s="31"/>
-      <c r="S1" s="120" t="s">
+      <c r="S1" s="122" t="s">
         <v>514</v>
       </c>
-      <c r="T1" s="121"/>
-      <c r="U1" s="121"/>
-      <c r="V1" s="121"/>
-      <c r="W1" s="121"/>
-      <c r="X1" s="121"/>
-      <c r="Y1" s="122"/>
+      <c r="T1" s="123"/>
+      <c r="U1" s="123"/>
+      <c r="V1" s="123"/>
+      <c r="W1" s="123"/>
+      <c r="X1" s="123"/>
+      <c r="Y1" s="124"/>
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="31" t="s">
@@ -25308,10 +25355,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{443B9AFF-7BD6-4AE0-89E2-431DFFEF3C27}">
-  <dimension ref="A1:U49"/>
+  <dimension ref="A1:Z49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O5" activeCellId="1" sqref="O13 O5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26:O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25328,7 +25375,7 @@
     <col min="20" max="21" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:26">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
@@ -25379,13 +25426,19 @@
       </c>
       <c r="Q1" s="31"/>
       <c r="R1" s="31"/>
-      <c r="S1" s="123" t="s">
+      <c r="S1" s="125" t="s">
         <v>514</v>
       </c>
-      <c r="T1" s="123"/>
-      <c r="U1" s="124"/>
-    </row>
-    <row r="2" spans="1:21">
+      <c r="T1" s="126"/>
+      <c r="U1" s="127"/>
+      <c r="W1" s="128" t="s">
+        <v>489</v>
+      </c>
+      <c r="X1" s="129"/>
+      <c r="Y1" s="129"/>
+      <c r="Z1" s="130"/>
+    </row>
+    <row r="2" spans="1:26">
       <c r="A2" s="31" t="s">
         <v>48</v>
       </c>
@@ -25447,8 +25500,20 @@
       <c r="U2" s="113" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="3" spans="1:21">
+      <c r="W2" s="120" t="s">
+        <v>48</v>
+      </c>
+      <c r="X2" s="120" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y2" s="120" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z2" s="120" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
       <c r="A3" s="31" t="s">
         <v>48</v>
       </c>
@@ -25508,8 +25573,24 @@
       <c r="U3" s="91">
         <v>2.92</v>
       </c>
-    </row>
-    <row r="4" spans="1:21">
+      <c r="W3" s="121">
+        <f>AVERAGE(O2:O7,O26:O31)</f>
+        <v>3.2300000000000004</v>
+      </c>
+      <c r="X3" s="121">
+        <f>AVERAGE(O32:O40,O8:O13)</f>
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="Y3" s="121">
+        <f>AVERAGE(O14:O19,O41:O46)</f>
+        <v>2.9291666666666667</v>
+      </c>
+      <c r="Z3" s="121">
+        <f>AVERAGE(O20:O25,O47:O49)</f>
+        <v>3.523333333333333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4" s="31" t="s">
         <v>48</v>
       </c>
@@ -25564,7 +25645,7 @@
       <c r="T4" s="31"/>
       <c r="U4" s="31"/>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:26">
       <c r="A5" s="31" t="s">
         <v>48</v>
       </c>
@@ -25619,7 +25700,7 @@
       <c r="T5" s="31"/>
       <c r="U5" s="31"/>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:26">
       <c r="A6" s="45" t="s">
         <v>48</v>
       </c>
@@ -25672,7 +25753,7 @@
       <c r="T6" s="31"/>
       <c r="U6" s="31"/>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:26">
       <c r="A7" s="31" t="s">
         <v>48</v>
       </c>
@@ -25727,54 +25808,54 @@
       <c r="T7" s="31"/>
       <c r="U7" s="31"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:26">
       <c r="A8" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="110">
-        <v>45240</v>
+        <v>48</v>
+      </c>
+      <c r="B8" s="70">
+        <v>45037</v>
       </c>
       <c r="C8" s="71">
-        <v>0.42569444444444443</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="D8" s="31">
-        <v>30.9</v>
+        <v>11.9</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>448</v>
+        <v>21</v>
       </c>
       <c r="F8" s="31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="31" t="s">
-        <v>469</v>
-      </c>
-      <c r="H8" s="37">
-        <v>413487</v>
+        <v>49</v>
+      </c>
+      <c r="H8" s="31">
+        <v>141020</v>
       </c>
       <c r="I8" s="31" t="s">
-        <v>470</v>
-      </c>
-      <c r="J8" s="31" t="s">
-        <v>471</v>
+        <v>50</v>
+      </c>
+      <c r="J8" s="116" t="s">
+        <v>51</v>
       </c>
       <c r="K8" s="31">
-        <v>3.28</v>
-      </c>
-      <c r="L8" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="M8" s="31" t="s">
-        <v>472</v>
+        <v>3.14</v>
+      </c>
+      <c r="L8" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" s="31">
+        <v>43858</v>
       </c>
       <c r="N8" s="31" t="s">
-        <v>457</v>
+        <v>26</v>
       </c>
       <c r="O8" s="31">
-        <v>1.81</v>
+        <v>6.91</v>
       </c>
       <c r="P8" s="31" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="Q8" s="31"/>
       <c r="R8" s="31"/>
@@ -25782,54 +25863,52 @@
       <c r="T8" s="31"/>
       <c r="U8" s="31"/>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:26">
       <c r="A9" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="110">
-        <v>45240</v>
+        <v>48</v>
+      </c>
+      <c r="B9" s="70">
+        <v>45037</v>
       </c>
       <c r="C9" s="71">
-        <v>0.42569444444444443</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="D9" s="31">
-        <v>30.9</v>
+        <v>11.9</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>448</v>
+        <v>21</v>
       </c>
       <c r="F9" s="31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G9" s="31" t="s">
-        <v>469</v>
-      </c>
-      <c r="H9" s="37">
-        <v>413488</v>
+        <v>49</v>
+      </c>
+      <c r="H9" s="31">
+        <v>141021</v>
       </c>
       <c r="I9" s="31" t="s">
-        <v>470</v>
-      </c>
-      <c r="J9" s="31" t="s">
-        <v>471</v>
-      </c>
-      <c r="K9" s="31">
-        <v>3.23</v>
-      </c>
-      <c r="L9" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="M9" s="31" t="s">
-        <v>473</v>
+        <v>50</v>
+      </c>
+      <c r="J9" s="116" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="31">
+        <v>43845</v>
       </c>
       <c r="N9" s="31" t="s">
-        <v>457</v>
+        <v>26</v>
       </c>
       <c r="O9" s="31">
-        <v>2.19</v>
+        <v>5.03</v>
       </c>
       <c r="P9" s="31" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="Q9" s="31"/>
       <c r="R9" s="31"/>
@@ -25837,54 +25916,54 @@
       <c r="T9" s="31"/>
       <c r="U9" s="31"/>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:26">
       <c r="A10" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="110">
-        <v>45240</v>
+        <v>48</v>
+      </c>
+      <c r="B10" s="70">
+        <v>45037</v>
       </c>
       <c r="C10" s="71">
-        <v>0.42569444444444443</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="D10" s="31">
-        <v>30.9</v>
+        <v>11.9</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>448</v>
+        <v>21</v>
       </c>
       <c r="F10" s="31">
+        <v>1</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="31">
+        <v>141019</v>
+      </c>
+      <c r="I10" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="J10" s="116" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="31">
         <v>3</v>
       </c>
-      <c r="G10" s="31" t="s">
-        <v>469</v>
-      </c>
-      <c r="H10" s="37">
-        <v>413489</v>
-      </c>
-      <c r="I10" s="31" t="s">
-        <v>470</v>
-      </c>
-      <c r="J10" s="31" t="s">
-        <v>471</v>
-      </c>
-      <c r="K10" s="31">
-        <v>3.25</v>
-      </c>
-      <c r="L10" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="M10" s="31" t="s">
-        <v>474</v>
+      <c r="L10" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="M10" s="31">
+        <v>43840</v>
       </c>
       <c r="N10" s="31" t="s">
-        <v>457</v>
-      </c>
-      <c r="O10" s="31">
-        <v>2.62</v>
+        <v>26</v>
+      </c>
+      <c r="O10" s="60">
+        <v>6.6</v>
       </c>
       <c r="P10" s="31" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="Q10" s="31"/>
       <c r="R10" s="31"/>
@@ -25892,54 +25971,54 @@
       <c r="T10" s="31"/>
       <c r="U10" s="31"/>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:26">
       <c r="A11" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="110">
-        <v>45240</v>
+        <v>48</v>
+      </c>
+      <c r="B11" s="70">
+        <v>45037</v>
       </c>
       <c r="C11" s="71">
-        <v>0.42569444444444443</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="D11" s="31">
-        <v>30.9</v>
+        <v>11.9</v>
       </c>
       <c r="E11" s="31" t="s">
         <v>63</v>
       </c>
       <c r="F11" s="31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" s="31" t="s">
-        <v>469</v>
-      </c>
-      <c r="H11" s="37">
-        <v>413490</v>
+        <v>49</v>
+      </c>
+      <c r="H11" s="31">
+        <v>141023</v>
       </c>
       <c r="I11" s="31" t="s">
-        <v>470</v>
-      </c>
-      <c r="J11" s="31" t="s">
-        <v>471</v>
+        <v>50</v>
+      </c>
+      <c r="J11" s="116" t="s">
+        <v>51</v>
       </c>
       <c r="K11" s="31">
-        <v>3.25</v>
-      </c>
-      <c r="L11" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="M11" s="31" t="s">
-        <v>475</v>
+        <v>3.02</v>
+      </c>
+      <c r="L11" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" s="31">
+        <v>43857</v>
       </c>
       <c r="N11" s="31" t="s">
-        <v>457</v>
+        <v>26</v>
       </c>
       <c r="O11" s="31">
-        <v>4.3099999999999996</v>
+        <v>3.28</v>
       </c>
       <c r="P11" s="31" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="Q11" s="31"/>
       <c r="R11" s="31"/>
@@ -25947,54 +26026,54 @@
       <c r="T11" s="31"/>
       <c r="U11" s="31"/>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:26">
       <c r="A12" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="110">
-        <v>45240</v>
+        <v>48</v>
+      </c>
+      <c r="B12" s="70">
+        <v>45037</v>
       </c>
       <c r="C12" s="71">
-        <v>0.42569444444444443</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="D12" s="31">
-        <v>30.9</v>
+        <v>11.9</v>
       </c>
       <c r="E12" s="31" t="s">
         <v>63</v>
       </c>
       <c r="F12" s="31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G12" s="31" t="s">
-        <v>469</v>
-      </c>
-      <c r="H12" s="37">
-        <v>413491</v>
+        <v>49</v>
+      </c>
+      <c r="H12" s="31">
+        <v>141024</v>
       </c>
       <c r="I12" s="31" t="s">
-        <v>470</v>
-      </c>
-      <c r="J12" s="31" t="s">
-        <v>471</v>
+        <v>50</v>
+      </c>
+      <c r="J12" s="116" t="s">
+        <v>51</v>
       </c>
       <c r="K12" s="31">
-        <v>3.31</v>
-      </c>
-      <c r="L12" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="M12" s="31" t="s">
-        <v>476</v>
+        <v>3</v>
+      </c>
+      <c r="L12" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" s="31">
+        <v>43852</v>
       </c>
       <c r="N12" s="31" t="s">
-        <v>457</v>
+        <v>26</v>
       </c>
       <c r="O12" s="31">
-        <v>3.78</v>
+        <v>2.63</v>
       </c>
       <c r="P12" s="31" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="Q12" s="31"/>
       <c r="R12" s="31"/>
@@ -26002,52 +26081,54 @@
       <c r="T12" s="31"/>
       <c r="U12" s="31"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:26">
       <c r="A13" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="110">
-        <v>45240</v>
+        <v>48</v>
+      </c>
+      <c r="B13" s="70">
+        <v>45037</v>
       </c>
       <c r="C13" s="71">
-        <v>0.42569444444444443</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="D13" s="31">
-        <v>30.9</v>
+        <v>11.9</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>63</v>
       </c>
       <c r="F13" s="31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>469</v>
-      </c>
-      <c r="H13" s="37">
-        <v>413492</v>
+        <v>49</v>
+      </c>
+      <c r="H13" s="31">
+        <v>141022</v>
       </c>
       <c r="I13" s="31" t="s">
-        <v>470</v>
-      </c>
-      <c r="J13" s="31" t="s">
-        <v>471</v>
-      </c>
-      <c r="K13" s="31"/>
-      <c r="L13" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="M13" s="31" t="s">
-        <v>477</v>
+        <v>50</v>
+      </c>
+      <c r="J13" s="116" t="s">
+        <v>51</v>
+      </c>
+      <c r="K13" s="31">
+        <v>3.04</v>
+      </c>
+      <c r="L13" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="M13" s="31">
+        <v>43850</v>
       </c>
       <c r="N13" s="31" t="s">
-        <v>457</v>
-      </c>
-      <c r="O13" s="60">
-        <v>2.7</v>
+        <v>26</v>
+      </c>
+      <c r="O13" s="31">
+        <v>4.3899999999999997</v>
       </c>
       <c r="P13" s="31" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="Q13" s="31"/>
       <c r="R13" s="31"/>
@@ -26055,18 +26136,18 @@
       <c r="T13" s="31"/>
       <c r="U13" s="31"/>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:26">
       <c r="A14" s="31" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B14" s="110">
         <v>45240</v>
       </c>
       <c r="C14" s="71">
-        <v>0.38958333333333334</v>
+        <v>0.42569444444444443</v>
       </c>
       <c r="D14" s="31">
-        <v>74</v>
+        <v>30.9</v>
       </c>
       <c r="E14" s="31" t="s">
         <v>448</v>
@@ -26075,31 +26156,31 @@
         <v>1</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>460</v>
+        <v>469</v>
       </c>
       <c r="H14" s="37">
-        <v>413481</v>
+        <v>413487</v>
       </c>
       <c r="I14" s="31" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
       <c r="J14" s="31" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
       <c r="K14" s="31">
-        <v>3.31</v>
+        <v>3.28</v>
       </c>
       <c r="L14" s="72" t="s">
         <v>25</v>
       </c>
       <c r="M14" s="31" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
       <c r="N14" s="31" t="s">
         <v>457</v>
       </c>
       <c r="O14" s="31">
-        <v>1.88</v>
+        <v>1.81</v>
       </c>
       <c r="P14" s="31" t="s">
         <v>93</v>
@@ -26110,18 +26191,18 @@
       <c r="T14" s="31"/>
       <c r="U14" s="31"/>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:26">
       <c r="A15" s="31" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B15" s="110">
         <v>45240</v>
       </c>
       <c r="C15" s="71">
-        <v>0.38958333333333334</v>
+        <v>0.42569444444444443</v>
       </c>
       <c r="D15" s="31">
-        <v>74</v>
+        <v>30.9</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>448</v>
@@ -26130,31 +26211,31 @@
         <v>2</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>460</v>
+        <v>469</v>
       </c>
       <c r="H15" s="37">
-        <v>413482</v>
+        <v>413488</v>
       </c>
       <c r="I15" s="31" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
       <c r="J15" s="31" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
       <c r="K15" s="31">
-        <v>3.26</v>
+        <v>3.23</v>
       </c>
       <c r="L15" s="72" t="s">
         <v>25</v>
       </c>
       <c r="M15" s="31" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
       <c r="N15" s="31" t="s">
         <v>457</v>
       </c>
       <c r="O15" s="31">
-        <v>1.33</v>
+        <v>2.19</v>
       </c>
       <c r="P15" s="31" t="s">
         <v>93</v>
@@ -26165,18 +26246,18 @@
       <c r="T15" s="31"/>
       <c r="U15" s="31"/>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:26">
       <c r="A16" s="31" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B16" s="110">
         <v>45240</v>
       </c>
       <c r="C16" s="71">
-        <v>0.38958333333333334</v>
+        <v>0.42569444444444443</v>
       </c>
       <c r="D16" s="31">
-        <v>74</v>
+        <v>30.9</v>
       </c>
       <c r="E16" s="31" t="s">
         <v>448</v>
@@ -26185,31 +26266,31 @@
         <v>3</v>
       </c>
       <c r="G16" s="31" t="s">
-        <v>460</v>
+        <v>469</v>
       </c>
       <c r="H16" s="37">
-        <v>413483</v>
+        <v>413489</v>
       </c>
       <c r="I16" s="31" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
       <c r="J16" s="31" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
       <c r="K16" s="31">
-        <v>3.2</v>
+        <v>3.25</v>
       </c>
       <c r="L16" s="72" t="s">
         <v>25</v>
       </c>
       <c r="M16" s="31" t="s">
-        <v>465</v>
+        <v>474</v>
       </c>
       <c r="N16" s="31" t="s">
         <v>457</v>
       </c>
       <c r="O16" s="31">
-        <v>2.27</v>
+        <v>2.62</v>
       </c>
       <c r="P16" s="31" t="s">
         <v>93</v>
@@ -26222,16 +26303,16 @@
     </row>
     <row r="17" spans="1:21">
       <c r="A17" s="31" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B17" s="110">
         <v>45240</v>
       </c>
       <c r="C17" s="71">
-        <v>0.38958333333333334</v>
+        <v>0.42569444444444443</v>
       </c>
       <c r="D17" s="31">
-        <v>74</v>
+        <v>30.9</v>
       </c>
       <c r="E17" s="31" t="s">
         <v>63</v>
@@ -26240,31 +26321,31 @@
         <v>1</v>
       </c>
       <c r="G17" s="31" t="s">
-        <v>460</v>
+        <v>469</v>
       </c>
       <c r="H17" s="37">
-        <v>413484</v>
+        <v>413490</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
       <c r="J17" s="31" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
       <c r="K17" s="31">
-        <v>3.22</v>
+        <v>3.25</v>
       </c>
       <c r="L17" s="72" t="s">
         <v>25</v>
       </c>
       <c r="M17" s="31" t="s">
-        <v>466</v>
+        <v>475</v>
       </c>
       <c r="N17" s="31" t="s">
         <v>457</v>
       </c>
-      <c r="O17" s="60">
-        <v>4.7</v>
+      <c r="O17" s="31">
+        <v>4.3099999999999996</v>
       </c>
       <c r="P17" s="31" t="s">
         <v>93</v>
@@ -26277,16 +26358,16 @@
     </row>
     <row r="18" spans="1:21">
       <c r="A18" s="31" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B18" s="110">
         <v>45240</v>
       </c>
       <c r="C18" s="71">
-        <v>0.38958333333333334</v>
+        <v>0.42569444444444443</v>
       </c>
       <c r="D18" s="31">
-        <v>74</v>
+        <v>30.9</v>
       </c>
       <c r="E18" s="31" t="s">
         <v>63</v>
@@ -26295,31 +26376,31 @@
         <v>2</v>
       </c>
       <c r="G18" s="31" t="s">
-        <v>460</v>
+        <v>469</v>
       </c>
       <c r="H18" s="37">
-        <v>413485</v>
+        <v>413491</v>
       </c>
       <c r="I18" s="31" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
       <c r="J18" s="31" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
       <c r="K18" s="31">
-        <v>3.21</v>
+        <v>3.31</v>
       </c>
       <c r="L18" s="72" t="s">
         <v>25</v>
       </c>
       <c r="M18" s="31" t="s">
-        <v>467</v>
+        <v>476</v>
       </c>
       <c r="N18" s="31" t="s">
         <v>457</v>
       </c>
       <c r="O18" s="31">
-        <v>3.82</v>
+        <v>3.78</v>
       </c>
       <c r="P18" s="31" t="s">
         <v>93</v>
@@ -26332,7 +26413,7 @@
     </row>
     <row r="19" spans="1:21">
       <c r="A19" s="31" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B19" s="110">
         <v>45240</v>
@@ -26341,7 +26422,7 @@
         <v>0.42569444444444443</v>
       </c>
       <c r="D19" s="31">
-        <v>74</v>
+        <v>30.9</v>
       </c>
       <c r="E19" s="31" t="s">
         <v>63</v>
@@ -26350,31 +26431,29 @@
         <v>3</v>
       </c>
       <c r="G19" s="31" t="s">
-        <v>460</v>
+        <v>469</v>
       </c>
       <c r="H19" s="37">
-        <v>413486</v>
+        <v>413492</v>
       </c>
       <c r="I19" s="31" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
       <c r="J19" s="31" t="s">
-        <v>462</v>
-      </c>
-      <c r="K19" s="31">
-        <v>3.23</v>
-      </c>
+        <v>471</v>
+      </c>
+      <c r="K19" s="31"/>
       <c r="L19" s="72" t="s">
         <v>25</v>
       </c>
       <c r="M19" s="31" t="s">
-        <v>468</v>
+        <v>477</v>
       </c>
       <c r="N19" s="31" t="s">
         <v>457</v>
       </c>
-      <c r="O19" s="31">
-        <v>2.41</v>
+      <c r="O19" s="60">
+        <v>2.7</v>
       </c>
       <c r="P19" s="31" t="s">
         <v>93</v>
@@ -26387,50 +26466,50 @@
     </row>
     <row r="20" spans="1:21">
       <c r="A20" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="110">
-        <v>45240</v>
+        <v>43</v>
+      </c>
+      <c r="B20" s="70">
+        <v>45037</v>
       </c>
       <c r="C20" s="71">
-        <v>0.35208333333333336</v>
+        <v>0.45902777777777776</v>
       </c>
       <c r="D20" s="31">
-        <v>112</v>
+        <v>31.7</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>448</v>
-      </c>
-      <c r="F20" s="115">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="F20" s="31">
+        <v>2</v>
       </c>
       <c r="G20" s="31" t="s">
-        <v>449</v>
-      </c>
-      <c r="H20" s="35">
-        <v>413475</v>
+        <v>44</v>
+      </c>
+      <c r="H20" s="31">
+        <v>141014</v>
       </c>
       <c r="I20" s="31" t="s">
-        <v>450</v>
-      </c>
-      <c r="J20" s="31" t="s">
-        <v>451</v>
-      </c>
-      <c r="K20" s="115"/>
-      <c r="L20" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="M20" s="31" t="s">
-        <v>452</v>
+        <v>45</v>
+      </c>
+      <c r="J20" s="116" t="s">
+        <v>46</v>
+      </c>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="31">
+        <v>43842</v>
       </c>
       <c r="N20" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="O20" s="31">
-        <v>2.3199999999999998</v>
+        <v>26</v>
+      </c>
+      <c r="O20" s="60">
+        <v>2.8</v>
       </c>
       <c r="P20" s="31" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="Q20" s="31"/>
       <c r="R20" s="31"/>
@@ -26440,50 +26519,52 @@
     </row>
     <row r="21" spans="1:21">
       <c r="A21" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="110">
-        <v>45240</v>
+        <v>43</v>
+      </c>
+      <c r="B21" s="70">
+        <v>45037</v>
       </c>
       <c r="C21" s="71">
-        <v>0.35208333333333336</v>
+        <v>0.45902777777777776</v>
       </c>
       <c r="D21" s="31">
-        <v>112</v>
+        <v>31.7</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>448</v>
+        <v>21</v>
       </c>
       <c r="F21" s="31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>449</v>
-      </c>
-      <c r="H21" s="35">
-        <v>413476</v>
+        <v>44</v>
+      </c>
+      <c r="H21" s="31">
+        <v>141013</v>
       </c>
       <c r="I21" s="31" t="s">
-        <v>450</v>
-      </c>
-      <c r="J21" s="31" t="s">
-        <v>451</v>
-      </c>
-      <c r="K21" s="31"/>
-      <c r="L21" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="M21" s="31" t="s">
-        <v>454</v>
+        <v>45</v>
+      </c>
+      <c r="J21" s="116" t="s">
+        <v>46</v>
+      </c>
+      <c r="K21" s="31">
+        <v>1.75</v>
+      </c>
+      <c r="L21" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="M21" s="31">
+        <v>43853</v>
       </c>
       <c r="N21" s="31" t="s">
-        <v>92</v>
+        <v>26</v>
       </c>
       <c r="O21" s="31">
-        <v>1.79</v>
+        <v>3.41</v>
       </c>
       <c r="P21" s="31" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="Q21" s="31"/>
       <c r="R21" s="31"/>
@@ -26493,50 +26574,52 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="110">
-        <v>45240</v>
+        <v>43</v>
+      </c>
+      <c r="B22" s="70">
+        <v>45037</v>
       </c>
       <c r="C22" s="71">
-        <v>0.35208333333333336</v>
+        <v>0.45902777777777776</v>
       </c>
       <c r="D22" s="31">
-        <v>112</v>
+        <v>31.7</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>448</v>
+        <v>21</v>
       </c>
       <c r="F22" s="31">
         <v>3</v>
       </c>
       <c r="G22" s="31" t="s">
-        <v>449</v>
-      </c>
-      <c r="H22" s="35">
-        <v>413477</v>
+        <v>44</v>
+      </c>
+      <c r="H22" s="31">
+        <v>141015</v>
       </c>
       <c r="I22" s="31" t="s">
-        <v>450</v>
-      </c>
-      <c r="J22" s="31" t="s">
-        <v>451</v>
-      </c>
-      <c r="K22" s="31"/>
-      <c r="L22" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="M22" s="31" t="s">
-        <v>455</v>
+        <v>45</v>
+      </c>
+      <c r="J22" s="116" t="s">
+        <v>46</v>
+      </c>
+      <c r="K22" s="31">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L22" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="M22" s="31">
+        <v>43855</v>
       </c>
       <c r="N22" s="31" t="s">
-        <v>92</v>
+        <v>26</v>
       </c>
       <c r="O22" s="31">
-        <v>2.23</v>
+        <v>3.82</v>
       </c>
       <c r="P22" s="31" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="Q22" s="31"/>
       <c r="R22" s="31"/>
@@ -26546,49 +26629,49 @@
     </row>
     <row r="23" spans="1:21">
       <c r="A23" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="110">
-        <v>45240</v>
+        <v>43</v>
+      </c>
+      <c r="B23" s="70">
+        <v>45149</v>
       </c>
       <c r="C23" s="71">
-        <v>0.35208333333333336</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="D23" s="31">
-        <v>112</v>
+        <v>34.5</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="F23" s="31">
         <v>1</v>
       </c>
       <c r="G23" s="31" t="s">
-        <v>449</v>
-      </c>
-      <c r="H23" s="37">
-        <v>413478</v>
+        <v>95</v>
+      </c>
+      <c r="H23" s="35">
+        <v>413322</v>
       </c>
       <c r="I23" s="31" t="s">
-        <v>450</v>
+        <v>96</v>
       </c>
       <c r="J23" s="31" t="s">
-        <v>451</v>
+        <v>97</v>
       </c>
       <c r="K23" s="31">
-        <v>3.25</v>
+        <v>3.4</v>
       </c>
       <c r="L23" s="72" t="s">
         <v>25</v>
       </c>
       <c r="M23" s="31" t="s">
-        <v>456</v>
+        <v>98</v>
       </c>
       <c r="N23" s="31" t="s">
-        <v>457</v>
+        <v>92</v>
       </c>
       <c r="O23" s="31">
-        <v>3.83</v>
+        <v>2.27</v>
       </c>
       <c r="P23" s="31" t="s">
         <v>93</v>
@@ -26601,49 +26684,49 @@
     </row>
     <row r="24" spans="1:21">
       <c r="A24" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="110">
-        <v>45240</v>
+        <v>43</v>
+      </c>
+      <c r="B24" s="70">
+        <v>45149</v>
       </c>
       <c r="C24" s="71">
-        <v>0.35208333333333336</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="D24" s="31">
-        <v>112</v>
+        <v>34.5</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="F24" s="31">
         <v>2</v>
       </c>
       <c r="G24" s="31" t="s">
-        <v>449</v>
-      </c>
-      <c r="H24" s="37">
-        <v>413479</v>
+        <v>95</v>
+      </c>
+      <c r="H24" s="35">
+        <v>413323</v>
       </c>
       <c r="I24" s="31" t="s">
-        <v>450</v>
+        <v>96</v>
       </c>
       <c r="J24" s="31" t="s">
-        <v>451</v>
+        <v>97</v>
       </c>
       <c r="K24" s="31">
-        <v>3.23</v>
+        <v>3.6</v>
       </c>
       <c r="L24" s="72" t="s">
         <v>25</v>
       </c>
       <c r="M24" s="31" t="s">
-        <v>458</v>
+        <v>100</v>
       </c>
       <c r="N24" s="31" t="s">
-        <v>457</v>
+        <v>92</v>
       </c>
       <c r="O24" s="60">
-        <v>3.2</v>
+        <v>3.8</v>
       </c>
       <c r="P24" s="31" t="s">
         <v>93</v>
@@ -26656,49 +26739,49 @@
     </row>
     <row r="25" spans="1:21">
       <c r="A25" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="110">
-        <v>45240</v>
+        <v>43</v>
+      </c>
+      <c r="B25" s="70">
+        <v>45149</v>
       </c>
       <c r="C25" s="71">
-        <v>0.35208333333333336</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="D25" s="31">
-        <v>112</v>
+        <v>34.5</v>
       </c>
       <c r="E25" s="31" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="F25" s="31">
         <v>3</v>
       </c>
       <c r="G25" s="31" t="s">
-        <v>449</v>
-      </c>
-      <c r="H25" s="37">
-        <v>413480</v>
+        <v>95</v>
+      </c>
+      <c r="H25" s="35">
+        <v>413324</v>
       </c>
       <c r="I25" s="31" t="s">
-        <v>450</v>
+        <v>96</v>
       </c>
       <c r="J25" s="31" t="s">
-        <v>451</v>
+        <v>97</v>
       </c>
       <c r="K25" s="31">
-        <v>3.18</v>
+        <v>3.22</v>
       </c>
       <c r="L25" s="72" t="s">
         <v>25</v>
       </c>
       <c r="M25" s="31" t="s">
-        <v>459</v>
+        <v>102</v>
       </c>
       <c r="N25" s="31" t="s">
-        <v>457</v>
+        <v>92</v>
       </c>
       <c r="O25" s="31">
-        <v>4.37</v>
+        <v>3.45</v>
       </c>
       <c r="P25" s="31" t="s">
         <v>93</v>
@@ -26711,49 +26794,49 @@
     </row>
     <row r="26" spans="1:21">
       <c r="A26" s="31" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B26" s="70">
         <v>45037</v>
       </c>
       <c r="C26" s="71">
-        <v>0.52500000000000002</v>
+        <v>0.45902777777777776</v>
       </c>
       <c r="D26" s="31">
-        <v>11.9</v>
+        <v>31.7</v>
       </c>
       <c r="E26" s="31" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="F26" s="31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G26" s="31" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H26" s="31">
-        <v>141020</v>
+        <v>141016</v>
       </c>
       <c r="I26" s="31" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J26" s="116" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="K26" s="31">
-        <v>3.14</v>
+        <v>3</v>
       </c>
       <c r="L26" s="31" t="s">
         <v>25</v>
       </c>
       <c r="M26" s="31">
-        <v>43858</v>
+        <v>43860</v>
       </c>
       <c r="N26" s="31" t="s">
         <v>26</v>
       </c>
       <c r="O26" s="31">
-        <v>6.91</v>
+        <v>4.71</v>
       </c>
       <c r="P26" s="31" t="s">
         <v>27</v>
@@ -26766,47 +26849,49 @@
     </row>
     <row r="27" spans="1:21">
       <c r="A27" s="31" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B27" s="70">
         <v>45037</v>
       </c>
       <c r="C27" s="71">
-        <v>0.52500000000000002</v>
+        <v>0.45902777777777776</v>
       </c>
       <c r="D27" s="31">
-        <v>11.9</v>
+        <v>31.7</v>
       </c>
       <c r="E27" s="31" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="F27" s="31">
         <v>3</v>
       </c>
       <c r="G27" s="31" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H27" s="31">
-        <v>141021</v>
+        <v>141018</v>
       </c>
       <c r="I27" s="31" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J27" s="116" t="s">
-        <v>51</v>
-      </c>
-      <c r="K27" s="31"/>
+        <v>46</v>
+      </c>
+      <c r="K27" s="31">
+        <v>3.07</v>
+      </c>
       <c r="L27" s="31" t="s">
         <v>25</v>
       </c>
       <c r="M27" s="31">
-        <v>43845</v>
+        <v>43859</v>
       </c>
       <c r="N27" s="31" t="s">
         <v>26</v>
       </c>
       <c r="O27" s="31">
-        <v>5.03</v>
+        <v>4.93</v>
       </c>
       <c r="P27" s="31" t="s">
         <v>27</v>
@@ -26819,49 +26904,49 @@
     </row>
     <row r="28" spans="1:21">
       <c r="A28" s="31" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B28" s="70">
         <v>45037</v>
       </c>
       <c r="C28" s="71">
-        <v>0.52500000000000002</v>
+        <v>0.45902777777777776</v>
       </c>
       <c r="D28" s="31">
-        <v>11.9</v>
+        <v>31.7</v>
       </c>
       <c r="E28" s="31" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="F28" s="31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G28" s="31" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H28" s="31">
-        <v>141019</v>
+        <v>141017</v>
       </c>
       <c r="I28" s="31" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J28" s="116" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="K28" s="31">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="L28" s="31" t="s">
         <v>54</v>
       </c>
       <c r="M28" s="31">
-        <v>43840</v>
+        <v>43841</v>
       </c>
       <c r="N28" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="O28" s="60">
-        <v>6.6</v>
+      <c r="O28" s="31">
+        <v>5.07</v>
       </c>
       <c r="P28" s="31" t="s">
         <v>27</v>
@@ -26874,52 +26959,52 @@
     </row>
     <row r="29" spans="1:21">
       <c r="A29" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="70">
-        <v>45037</v>
+        <v>36</v>
+      </c>
+      <c r="B29" s="110">
+        <v>45240</v>
       </c>
       <c r="C29" s="71">
-        <v>0.52500000000000002</v>
+        <v>0.38958333333333334</v>
       </c>
       <c r="D29" s="31">
-        <v>11.9</v>
+        <v>74</v>
       </c>
       <c r="E29" s="31" t="s">
-        <v>63</v>
+        <v>448</v>
       </c>
       <c r="F29" s="31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G29" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="H29" s="31">
-        <v>141023</v>
+        <v>460</v>
+      </c>
+      <c r="H29" s="37">
+        <v>413481</v>
       </c>
       <c r="I29" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="J29" s="116" t="s">
-        <v>51</v>
+        <v>461</v>
+      </c>
+      <c r="J29" s="31" t="s">
+        <v>462</v>
       </c>
       <c r="K29" s="31">
-        <v>3.02</v>
-      </c>
-      <c r="L29" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="M29" s="31">
-        <v>43857</v>
+        <v>3.31</v>
+      </c>
+      <c r="L29" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="M29" s="31" t="s">
+        <v>463</v>
       </c>
       <c r="N29" s="31" t="s">
-        <v>26</v>
+        <v>457</v>
       </c>
       <c r="O29" s="31">
-        <v>3.28</v>
+        <v>1.88</v>
       </c>
       <c r="P29" s="31" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="Q29" s="31"/>
       <c r="R29" s="31"/>
@@ -26929,52 +27014,52 @@
     </row>
     <row r="30" spans="1:21">
       <c r="A30" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="B30" s="70">
-        <v>45037</v>
+        <v>36</v>
+      </c>
+      <c r="B30" s="110">
+        <v>45240</v>
       </c>
       <c r="C30" s="71">
-        <v>0.52500000000000002</v>
+        <v>0.38958333333333334</v>
       </c>
       <c r="D30" s="31">
-        <v>11.9</v>
+        <v>74</v>
       </c>
       <c r="E30" s="31" t="s">
-        <v>63</v>
+        <v>448</v>
       </c>
       <c r="F30" s="31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G30" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="H30" s="31">
-        <v>141024</v>
+        <v>460</v>
+      </c>
+      <c r="H30" s="37">
+        <v>413482</v>
       </c>
       <c r="I30" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="J30" s="116" t="s">
-        <v>51</v>
+        <v>461</v>
+      </c>
+      <c r="J30" s="31" t="s">
+        <v>462</v>
       </c>
       <c r="K30" s="31">
-        <v>3</v>
-      </c>
-      <c r="L30" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="M30" s="31">
-        <v>43852</v>
+        <v>3.26</v>
+      </c>
+      <c r="L30" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="M30" s="31" t="s">
+        <v>464</v>
       </c>
       <c r="N30" s="31" t="s">
-        <v>26</v>
+        <v>457</v>
       </c>
       <c r="O30" s="31">
-        <v>2.63</v>
+        <v>1.33</v>
       </c>
       <c r="P30" s="31" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="Q30" s="31"/>
       <c r="R30" s="31"/>
@@ -26984,52 +27069,52 @@
     </row>
     <row r="31" spans="1:21">
       <c r="A31" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="B31" s="70">
-        <v>45037</v>
+        <v>36</v>
+      </c>
+      <c r="B31" s="110">
+        <v>45240</v>
       </c>
       <c r="C31" s="71">
-        <v>0.52500000000000002</v>
+        <v>0.38958333333333334</v>
       </c>
       <c r="D31" s="31">
-        <v>11.9</v>
+        <v>74</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>63</v>
+        <v>448</v>
       </c>
       <c r="F31" s="31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G31" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="H31" s="31">
-        <v>141022</v>
+        <v>460</v>
+      </c>
+      <c r="H31" s="37">
+        <v>413483</v>
       </c>
       <c r="I31" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="J31" s="116" t="s">
-        <v>51</v>
+        <v>461</v>
+      </c>
+      <c r="J31" s="31" t="s">
+        <v>462</v>
       </c>
       <c r="K31" s="31">
-        <v>3.04</v>
-      </c>
-      <c r="L31" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="M31" s="31">
-        <v>43850</v>
+        <v>3.2</v>
+      </c>
+      <c r="L31" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="M31" s="31" t="s">
+        <v>465</v>
       </c>
       <c r="N31" s="31" t="s">
-        <v>26</v>
+        <v>457</v>
       </c>
       <c r="O31" s="31">
-        <v>4.3899999999999997</v>
+        <v>2.27</v>
       </c>
       <c r="P31" s="31" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="Q31" s="31"/>
       <c r="R31" s="31"/>
@@ -27039,50 +27124,52 @@
     </row>
     <row r="32" spans="1:21">
       <c r="A32" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="70">
-        <v>45037</v>
+        <v>36</v>
+      </c>
+      <c r="B32" s="110">
+        <v>45240</v>
       </c>
       <c r="C32" s="71">
-        <v>0.45902777777777776</v>
+        <v>0.38958333333333334</v>
       </c>
       <c r="D32" s="31">
-        <v>31.7</v>
+        <v>74</v>
       </c>
       <c r="E32" s="31" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="F32" s="31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G32" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="H32" s="31">
-        <v>141014</v>
+        <v>460</v>
+      </c>
+      <c r="H32" s="37">
+        <v>413484</v>
       </c>
       <c r="I32" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="J32" s="116" t="s">
-        <v>46</v>
-      </c>
-      <c r="K32" s="31"/>
-      <c r="L32" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="M32" s="31">
-        <v>43842</v>
+        <v>461</v>
+      </c>
+      <c r="J32" s="31" t="s">
+        <v>462</v>
+      </c>
+      <c r="K32" s="31">
+        <v>3.22</v>
+      </c>
+      <c r="L32" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="M32" s="31" t="s">
+        <v>466</v>
       </c>
       <c r="N32" s="31" t="s">
-        <v>26</v>
+        <v>457</v>
       </c>
       <c r="O32" s="60">
-        <v>2.8</v>
+        <v>4.7</v>
       </c>
       <c r="P32" s="31" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="Q32" s="31"/>
       <c r="R32" s="31"/>
@@ -27092,52 +27179,52 @@
     </row>
     <row r="33" spans="1:21">
       <c r="A33" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="70">
-        <v>45037</v>
+        <v>36</v>
+      </c>
+      <c r="B33" s="110">
+        <v>45240</v>
       </c>
       <c r="C33" s="71">
-        <v>0.45902777777777776</v>
+        <v>0.38958333333333334</v>
       </c>
       <c r="D33" s="31">
-        <v>31.7</v>
+        <v>74</v>
       </c>
       <c r="E33" s="31" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="F33" s="31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G33" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="H33" s="31">
-        <v>141013</v>
+        <v>460</v>
+      </c>
+      <c r="H33" s="37">
+        <v>413485</v>
       </c>
       <c r="I33" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="J33" s="116" t="s">
-        <v>46</v>
+        <v>461</v>
+      </c>
+      <c r="J33" s="31" t="s">
+        <v>462</v>
       </c>
       <c r="K33" s="31">
-        <v>1.75</v>
-      </c>
-      <c r="L33" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="M33" s="31">
-        <v>43853</v>
+        <v>3.21</v>
+      </c>
+      <c r="L33" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="M33" s="31" t="s">
+        <v>467</v>
       </c>
       <c r="N33" s="31" t="s">
-        <v>26</v>
+        <v>457</v>
       </c>
       <c r="O33" s="31">
-        <v>3.41</v>
+        <v>3.82</v>
       </c>
       <c r="P33" s="31" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="Q33" s="31"/>
       <c r="R33" s="31"/>
@@ -27147,52 +27234,52 @@
     </row>
     <row r="34" spans="1:21">
       <c r="A34" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B34" s="70">
-        <v>45037</v>
+        <v>36</v>
+      </c>
+      <c r="B34" s="110">
+        <v>45240</v>
       </c>
       <c r="C34" s="71">
-        <v>0.45902777777777776</v>
+        <v>0.42569444444444443</v>
       </c>
       <c r="D34" s="31">
-        <v>31.7</v>
+        <v>74</v>
       </c>
       <c r="E34" s="31" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="F34" s="31">
         <v>3</v>
       </c>
       <c r="G34" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="H34" s="31">
-        <v>141015</v>
+        <v>460</v>
+      </c>
+      <c r="H34" s="37">
+        <v>413486</v>
       </c>
       <c r="I34" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="J34" s="116" t="s">
-        <v>46</v>
+        <v>461</v>
+      </c>
+      <c r="J34" s="31" t="s">
+        <v>462</v>
       </c>
       <c r="K34" s="31">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="L34" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="M34" s="31">
-        <v>43855</v>
+        <v>3.23</v>
+      </c>
+      <c r="L34" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="M34" s="31" t="s">
+        <v>468</v>
       </c>
       <c r="N34" s="31" t="s">
-        <v>26</v>
+        <v>457</v>
       </c>
       <c r="O34" s="31">
-        <v>3.82</v>
+        <v>2.41</v>
       </c>
       <c r="P34" s="31" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="Q34" s="31"/>
       <c r="R34" s="31"/>
@@ -27202,34 +27289,34 @@
     </row>
     <row r="35" spans="1:21">
       <c r="A35" s="31" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B35" s="70">
         <v>45037</v>
       </c>
       <c r="C35" s="71">
-        <v>0.45902777777777776</v>
+        <v>0.4152777777777778</v>
       </c>
       <c r="D35" s="31">
-        <v>31.7</v>
+        <v>77</v>
       </c>
       <c r="E35" s="31" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="F35" s="31">
         <v>1</v>
       </c>
       <c r="G35" s="31" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="H35" s="31">
-        <v>141016</v>
+        <v>141007</v>
       </c>
       <c r="I35" s="31" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J35" s="116" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="K35" s="31">
         <v>3</v>
@@ -27238,13 +27325,13 @@
         <v>25</v>
       </c>
       <c r="M35" s="31">
-        <v>43860</v>
+        <v>43849</v>
       </c>
       <c r="N35" s="31" t="s">
         <v>26</v>
       </c>
       <c r="O35" s="31">
-        <v>4.71</v>
+        <v>6.62</v>
       </c>
       <c r="P35" s="31" t="s">
         <v>27</v>
@@ -27257,49 +27344,49 @@
     </row>
     <row r="36" spans="1:21">
       <c r="A36" s="31" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B36" s="70">
         <v>45037</v>
       </c>
       <c r="C36" s="71">
-        <v>0.45902777777777776</v>
+        <v>0.4152777777777778</v>
       </c>
       <c r="D36" s="31">
-        <v>31.7</v>
+        <v>77</v>
       </c>
       <c r="E36" s="31" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="F36" s="31">
+        <v>2</v>
+      </c>
+      <c r="G36" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="H36" s="31">
+        <v>141008</v>
+      </c>
+      <c r="I36" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="J36" s="116" t="s">
+        <v>39</v>
+      </c>
+      <c r="K36" s="31">
         <v>3</v>
       </c>
-      <c r="G36" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="H36" s="31">
-        <v>141018</v>
-      </c>
-      <c r="I36" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="J36" s="116" t="s">
-        <v>46</v>
-      </c>
-      <c r="K36" s="31">
-        <v>3.07</v>
-      </c>
       <c r="L36" s="31" t="s">
         <v>25</v>
       </c>
       <c r="M36" s="31">
-        <v>43859</v>
+        <v>43844</v>
       </c>
       <c r="N36" s="31" t="s">
         <v>26</v>
       </c>
       <c r="O36" s="31">
-        <v>4.93</v>
+        <v>2.69</v>
       </c>
       <c r="P36" s="31" t="s">
         <v>27</v>
@@ -27312,49 +27399,49 @@
     </row>
     <row r="37" spans="1:21">
       <c r="A37" s="31" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B37" s="70">
         <v>45037</v>
       </c>
       <c r="C37" s="71">
-        <v>0.45902777777777776</v>
+        <v>0.4152777777777778</v>
       </c>
       <c r="D37" s="31">
-        <v>31.7</v>
+        <v>77</v>
       </c>
       <c r="E37" s="31" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="F37" s="31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G37" s="31" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="H37" s="31">
-        <v>141017</v>
+        <v>141009</v>
       </c>
       <c r="I37" s="31" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J37" s="116" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="K37" s="31">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="L37" s="31" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="M37" s="31">
-        <v>43841</v>
+        <v>43848</v>
       </c>
       <c r="N37" s="31" t="s">
         <v>26</v>
       </c>
       <c r="O37" s="31">
-        <v>5.07</v>
+        <v>4.38</v>
       </c>
       <c r="P37" s="31" t="s">
         <v>27</v>
@@ -27379,7 +27466,7 @@
         <v>77</v>
       </c>
       <c r="E38" s="31" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="F38" s="31">
         <v>1</v>
@@ -27388,7 +27475,7 @@
         <v>37</v>
       </c>
       <c r="H38" s="31">
-        <v>141007</v>
+        <v>141010</v>
       </c>
       <c r="I38" s="31" t="s">
         <v>38</v>
@@ -27397,19 +27484,19 @@
         <v>39</v>
       </c>
       <c r="K38" s="31">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="L38" s="31" t="s">
         <v>25</v>
       </c>
       <c r="M38" s="31">
-        <v>43849</v>
+        <v>43856</v>
       </c>
       <c r="N38" s="31" t="s">
         <v>26</v>
       </c>
       <c r="O38" s="31">
-        <v>6.62</v>
+        <v>3.68</v>
       </c>
       <c r="P38" s="31" t="s">
         <v>27</v>
@@ -27434,7 +27521,7 @@
         <v>77</v>
       </c>
       <c r="E39" s="31" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="F39" s="31">
         <v>2</v>
@@ -27443,7 +27530,7 @@
         <v>37</v>
       </c>
       <c r="H39" s="31">
-        <v>141008</v>
+        <v>141011</v>
       </c>
       <c r="I39" s="31" t="s">
         <v>38</v>
@@ -27452,19 +27539,19 @@
         <v>39</v>
       </c>
       <c r="K39" s="31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L39" s="31" t="s">
         <v>25</v>
       </c>
       <c r="M39" s="31">
-        <v>43844</v>
+        <v>43843</v>
       </c>
       <c r="N39" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="O39" s="31">
-        <v>2.69</v>
+      <c r="O39" s="60">
+        <v>3.8</v>
       </c>
       <c r="P39" s="31" t="s">
         <v>27</v>
@@ -27489,7 +27576,7 @@
         <v>77</v>
       </c>
       <c r="E40" s="31" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="F40" s="31">
         <v>3</v>
@@ -27498,7 +27585,7 @@
         <v>37</v>
       </c>
       <c r="H40" s="31">
-        <v>141009</v>
+        <v>141012</v>
       </c>
       <c r="I40" s="31" t="s">
         <v>38</v>
@@ -27507,19 +27594,19 @@
         <v>39</v>
       </c>
       <c r="K40" s="31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L40" s="31" t="s">
         <v>25</v>
       </c>
       <c r="M40" s="31">
-        <v>43848</v>
+        <v>43846</v>
       </c>
       <c r="N40" s="31" t="s">
         <v>26</v>
       </c>
       <c r="O40" s="31">
-        <v>4.38</v>
+        <v>4.46</v>
       </c>
       <c r="P40" s="31" t="s">
         <v>27</v>
@@ -27532,52 +27619,50 @@
     </row>
     <row r="41" spans="1:21">
       <c r="A41" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B41" s="70">
-        <v>45037</v>
+        <v>20</v>
+      </c>
+      <c r="B41" s="110">
+        <v>45240</v>
       </c>
       <c r="C41" s="71">
-        <v>0.4152777777777778</v>
+        <v>0.35208333333333336</v>
       </c>
       <c r="D41" s="31">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="E41" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="F41" s="31">
+        <v>448</v>
+      </c>
+      <c r="F41" s="115">
         <v>1</v>
       </c>
       <c r="G41" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="H41" s="31">
-        <v>141010</v>
+        <v>449</v>
+      </c>
+      <c r="H41" s="35">
+        <v>413475</v>
       </c>
       <c r="I41" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="J41" s="116" t="s">
-        <v>39</v>
-      </c>
-      <c r="K41" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="L41" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="M41" s="31">
-        <v>43856</v>
+        <v>450</v>
+      </c>
+      <c r="J41" s="31" t="s">
+        <v>451</v>
+      </c>
+      <c r="K41" s="115"/>
+      <c r="L41" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="M41" s="31" t="s">
+        <v>452</v>
       </c>
       <c r="N41" s="31" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
       <c r="O41" s="31">
-        <v>3.68</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="P41" s="31" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="Q41" s="31"/>
       <c r="R41" s="31"/>
@@ -27587,52 +27672,50 @@
     </row>
     <row r="42" spans="1:21">
       <c r="A42" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42" s="70">
-        <v>45037</v>
+        <v>20</v>
+      </c>
+      <c r="B42" s="110">
+        <v>45240</v>
       </c>
       <c r="C42" s="71">
-        <v>0.4152777777777778</v>
+        <v>0.35208333333333336</v>
       </c>
       <c r="D42" s="31">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="E42" s="31" t="s">
-        <v>63</v>
+        <v>448</v>
       </c>
       <c r="F42" s="31">
         <v>2</v>
       </c>
       <c r="G42" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="H42" s="31">
-        <v>141011</v>
+        <v>449</v>
+      </c>
+      <c r="H42" s="35">
+        <v>413476</v>
       </c>
       <c r="I42" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="J42" s="116" t="s">
-        <v>39</v>
-      </c>
-      <c r="K42" s="31">
-        <v>2</v>
-      </c>
-      <c r="L42" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="M42" s="31">
-        <v>43843</v>
+        <v>450</v>
+      </c>
+      <c r="J42" s="31" t="s">
+        <v>451</v>
+      </c>
+      <c r="K42" s="31"/>
+      <c r="L42" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="M42" s="31" t="s">
+        <v>454</v>
       </c>
       <c r="N42" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="O42" s="60">
-        <v>3.8</v>
+        <v>92</v>
+      </c>
+      <c r="O42" s="31">
+        <v>1.79</v>
       </c>
       <c r="P42" s="31" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="Q42" s="31"/>
       <c r="R42" s="31"/>
@@ -27642,52 +27725,50 @@
     </row>
     <row r="43" spans="1:21">
       <c r="A43" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B43" s="70">
-        <v>45037</v>
+        <v>20</v>
+      </c>
+      <c r="B43" s="110">
+        <v>45240</v>
       </c>
       <c r="C43" s="71">
-        <v>0.4152777777777778</v>
+        <v>0.35208333333333336</v>
       </c>
       <c r="D43" s="31">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="E43" s="31" t="s">
-        <v>63</v>
+        <v>448</v>
       </c>
       <c r="F43" s="31">
         <v>3</v>
       </c>
       <c r="G43" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="H43" s="31">
-        <v>141012</v>
+        <v>449</v>
+      </c>
+      <c r="H43" s="35">
+        <v>413477</v>
       </c>
       <c r="I43" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="J43" s="116" t="s">
-        <v>39</v>
-      </c>
-      <c r="K43" s="31">
-        <v>2</v>
-      </c>
-      <c r="L43" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="M43" s="31">
-        <v>43846</v>
+        <v>450</v>
+      </c>
+      <c r="J43" s="31" t="s">
+        <v>451</v>
+      </c>
+      <c r="K43" s="31"/>
+      <c r="L43" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="M43" s="31" t="s">
+        <v>455</v>
       </c>
       <c r="N43" s="31" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
       <c r="O43" s="31">
-        <v>4.46</v>
+        <v>2.23</v>
       </c>
       <c r="P43" s="31" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="Q43" s="31"/>
       <c r="R43" s="31"/>
@@ -27699,50 +27780,50 @@
       <c r="A44" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B44" s="70">
-        <v>45037</v>
+      <c r="B44" s="110">
+        <v>45240</v>
       </c>
       <c r="C44" s="71">
-        <v>0.35555555555555557</v>
+        <v>0.35208333333333336</v>
       </c>
       <c r="D44" s="31">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E44" s="31" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="F44" s="31">
         <v>1</v>
       </c>
       <c r="G44" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="H44" s="31">
-        <v>141001</v>
+        <v>449</v>
+      </c>
+      <c r="H44" s="37">
+        <v>413478</v>
       </c>
       <c r="I44" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="J44" s="116" t="s">
-        <v>24</v>
+        <v>450</v>
+      </c>
+      <c r="J44" s="31" t="s">
+        <v>451</v>
       </c>
       <c r="K44" s="31">
-        <v>3.5</v>
-      </c>
-      <c r="L44" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="M44" s="31">
-        <v>43854</v>
+        <v>3.25</v>
+      </c>
+      <c r="L44" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="M44" s="31" t="s">
+        <v>456</v>
       </c>
       <c r="N44" s="31" t="s">
-        <v>26</v>
+        <v>457</v>
       </c>
       <c r="O44" s="31">
-        <v>2.57</v>
+        <v>3.83</v>
       </c>
       <c r="P44" s="31" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="Q44" s="31"/>
       <c r="R44" s="31"/>
@@ -27754,50 +27835,50 @@
       <c r="A45" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B45" s="70">
-        <v>45037</v>
+      <c r="B45" s="110">
+        <v>45240</v>
       </c>
       <c r="C45" s="71">
-        <v>0.35555555555555557</v>
+        <v>0.35208333333333336</v>
       </c>
       <c r="D45" s="31">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E45" s="31" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="F45" s="31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G45" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="H45" s="31">
-        <v>141003</v>
+        <v>449</v>
+      </c>
+      <c r="H45" s="37">
+        <v>413479</v>
       </c>
       <c r="I45" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="J45" s="116" t="s">
-        <v>24</v>
+        <v>450</v>
+      </c>
+      <c r="J45" s="31" t="s">
+        <v>451</v>
       </c>
       <c r="K45" s="31">
-        <v>3.5</v>
-      </c>
-      <c r="L45" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="M45" s="31">
-        <v>43847</v>
+        <v>3.23</v>
+      </c>
+      <c r="L45" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="M45" s="31" t="s">
+        <v>458</v>
       </c>
       <c r="N45" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="O45" s="31">
-        <v>5.66</v>
+        <v>457</v>
+      </c>
+      <c r="O45" s="60">
+        <v>3.2</v>
       </c>
       <c r="P45" s="31" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="Q45" s="31"/>
       <c r="R45" s="31"/>
@@ -27809,50 +27890,50 @@
       <c r="A46" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B46" s="70">
-        <v>45037</v>
+      <c r="B46" s="110">
+        <v>45240</v>
       </c>
       <c r="C46" s="71">
-        <v>0.35555555555555557</v>
+        <v>0.35208333333333336</v>
       </c>
       <c r="D46" s="31">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E46" s="31" t="s">
         <v>63</v>
       </c>
       <c r="F46" s="31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G46" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="H46" s="31">
-        <v>141004</v>
+        <v>449</v>
+      </c>
+      <c r="H46" s="37">
+        <v>413480</v>
       </c>
       <c r="I46" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="J46" s="116" t="s">
-        <v>24</v>
+        <v>450</v>
+      </c>
+      <c r="J46" s="31" t="s">
+        <v>451</v>
       </c>
       <c r="K46" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="L46" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="M46" s="31">
-        <v>43851</v>
+        <v>3.18</v>
+      </c>
+      <c r="L46" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="M46" s="31" t="s">
+        <v>459</v>
       </c>
       <c r="N46" s="31" t="s">
-        <v>26</v>
+        <v>457</v>
       </c>
       <c r="O46" s="31">
-        <v>3.93</v>
+        <v>4.37</v>
       </c>
       <c r="P46" s="31" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="Q46" s="31"/>
       <c r="R46" s="31"/>
@@ -27862,16 +27943,16 @@
     </row>
     <row r="47" spans="1:21">
       <c r="A47" s="31" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="B47" s="70">
-        <v>45149</v>
+        <v>45037</v>
       </c>
       <c r="C47" s="71">
-        <v>0.39930555555555558</v>
+        <v>0.35555555555555557</v>
       </c>
       <c r="D47" s="31">
-        <v>34.5</v>
+        <v>114</v>
       </c>
       <c r="E47" s="31" t="s">
         <v>21</v>
@@ -27880,34 +27961,34 @@
         <v>1</v>
       </c>
       <c r="G47" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="H47" s="35">
-        <v>413322</v>
+        <v>22</v>
+      </c>
+      <c r="H47" s="31">
+        <v>141001</v>
       </c>
       <c r="I47" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="J47" s="31" t="s">
-        <v>97</v>
+        <v>23</v>
+      </c>
+      <c r="J47" s="116" t="s">
+        <v>24</v>
       </c>
       <c r="K47" s="31">
-        <v>3.4</v>
-      </c>
-      <c r="L47" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="M47" s="31" t="s">
-        <v>98</v>
+        <v>3.5</v>
+      </c>
+      <c r="L47" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="M47" s="31">
+        <v>43854</v>
       </c>
       <c r="N47" s="31" t="s">
-        <v>92</v>
+        <v>26</v>
       </c>
       <c r="O47" s="31">
-        <v>2.27</v>
+        <v>2.57</v>
       </c>
       <c r="P47" s="31" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="Q47" s="31"/>
       <c r="R47" s="31"/>
@@ -27917,52 +27998,52 @@
     </row>
     <row r="48" spans="1:21">
       <c r="A48" s="31" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="B48" s="70">
-        <v>45149</v>
+        <v>45037</v>
       </c>
       <c r="C48" s="71">
-        <v>0.39930555555555558</v>
+        <v>0.35555555555555557</v>
       </c>
       <c r="D48" s="31">
-        <v>34.5</v>
+        <v>114</v>
       </c>
       <c r="E48" s="31" t="s">
         <v>21</v>
       </c>
       <c r="F48" s="31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G48" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="H48" s="35">
-        <v>413323</v>
+        <v>22</v>
+      </c>
+      <c r="H48" s="31">
+        <v>141003</v>
       </c>
       <c r="I48" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="J48" s="31" t="s">
-        <v>97</v>
+        <v>23</v>
+      </c>
+      <c r="J48" s="116" t="s">
+        <v>24</v>
       </c>
       <c r="K48" s="31">
-        <v>3.6</v>
-      </c>
-      <c r="L48" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="M48" s="31" t="s">
-        <v>100</v>
+        <v>3.5</v>
+      </c>
+      <c r="L48" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="M48" s="31">
+        <v>43847</v>
       </c>
       <c r="N48" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="O48" s="60">
-        <v>3.8</v>
+        <v>26</v>
+      </c>
+      <c r="O48" s="31">
+        <v>5.66</v>
       </c>
       <c r="P48" s="31" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="Q48" s="31"/>
       <c r="R48" s="31"/>
@@ -27972,52 +28053,52 @@
     </row>
     <row r="49" spans="1:21">
       <c r="A49" s="31" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="B49" s="70">
-        <v>45149</v>
+        <v>45037</v>
       </c>
       <c r="C49" s="71">
-        <v>0.39930555555555558</v>
+        <v>0.35555555555555557</v>
       </c>
       <c r="D49" s="31">
-        <v>34.5</v>
+        <v>114</v>
       </c>
       <c r="E49" s="31" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="F49" s="31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G49" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="H49" s="35">
-        <v>413324</v>
+        <v>22</v>
+      </c>
+      <c r="H49" s="31">
+        <v>141004</v>
       </c>
       <c r="I49" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="J49" s="31" t="s">
-        <v>97</v>
+        <v>23</v>
+      </c>
+      <c r="J49" s="116" t="s">
+        <v>24</v>
       </c>
       <c r="K49" s="31">
-        <v>3.22</v>
-      </c>
-      <c r="L49" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="M49" s="31" t="s">
-        <v>102</v>
+        <v>1.5</v>
+      </c>
+      <c r="L49" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="M49" s="31">
+        <v>43851</v>
       </c>
       <c r="N49" s="31" t="s">
-        <v>92</v>
+        <v>26</v>
       </c>
       <c r="O49" s="31">
-        <v>3.45</v>
+        <v>3.93</v>
       </c>
       <c r="P49" s="31" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="Q49" s="31"/>
       <c r="R49" s="31"/>
@@ -28026,8 +28107,12 @@
       <c r="U49" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P49">
+    <sortCondition ref="A2:A49"/>
+  </sortState>
+  <mergeCells count="2">
     <mergeCell ref="S1:U1"/>
+    <mergeCell ref="W1:Z1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>